<commit_message>
correct sequential rot problem
</commit_message>
<xml_diff>
--- a/reference/css_matrix3d coordinates.xlsx
+++ b/reference/css_matrix3d coordinates.xlsx
@@ -5,16 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EP\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a88d59eb7980e77d/Families/30_Seanachan/桃園高中/自主學習計畫_Rubiks Cube Everywhere/10_學習過程記錄/30_Rubiks Cube by javascript/20_Code/Github/t907/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AD8DC7-6E3A-4971-AB1F-C81AE6AAD718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{80AD8DC7-6E3A-4971-AB1F-C81AE6AAD718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07E04537-3ECA-4733-9712-44C2DB5F79C4}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="17900" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$R$32</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -174,16 +177,106 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -600,10 +693,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:W31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
@@ -1114,24 +1210,24 @@
       <c r="A13" s="1"/>
       <c r="C13" s="10"/>
       <c r="D13" s="11" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE,D9:G12)</f>
-        <v>1, 0, 0, 0, 0, -1, 0, 0, 0, 0, -1, 0, 0, 0, 0, 1</v>
+        <f>"=matrix3d(" &amp; _xlfn.TEXTJOIN(", ", TRUE,D9:G12) &amp; ")"</f>
+        <v>=matrix3d(1, 0, 0, 0, 0, -1, 0, 0, 0, 0, -1, 0, 0, 0, 0, 1)</v>
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="1"/>
       <c r="I13" s="11" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE,I9:L12)</f>
-        <v>-1, 0, 0, 0, 0, 1, 0, 0, 0, 0, -1, 0, 0, 0, 0, 1</v>
+        <f>"=matrix3d(" &amp; _xlfn.TEXTJOIN(", ", TRUE,I9:L12) &amp; ")"</f>
+        <v>=matrix3d(-1, 0, 0, 0, 0, 1, 0, 0, 0, 0, -1, 0, 0, 0, 0, 1)</v>
       </c>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
       <c r="M13" s="1"/>
       <c r="N13" s="11" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE,N9:Q12)</f>
-        <v>-1, 0, 0, 0, 0, -1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1</v>
+        <f>"=matrix3d(" &amp; _xlfn.TEXTJOIN(", ", TRUE,N9:Q12) &amp; ")"</f>
+        <v>=matrix3d(-1, 0, 0, 0, 0, -1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1)</v>
       </c>
       <c r="O13" s="11"/>
       <c r="P13" s="11"/>
@@ -1383,24 +1479,24 @@
       <c r="A19" s="1"/>
       <c r="C19" s="10"/>
       <c r="D19" s="11" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE,D15:G18)</f>
-        <v>1, 0, 0, 0, 0, -1, 0, 0, 0, 0, -1, 0, 0, 0, 0, 1</v>
+        <f>"=matrix3d(" &amp; _xlfn.TEXTJOIN(", ", TRUE,D15:G18) &amp; ")"</f>
+        <v>=matrix3d(1, 0, 0, 0, 0, -1, 0, 0, 0, 0, -1, 0, 0, 0, 0, 1)</v>
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="1"/>
       <c r="I19" s="11" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE,I15:L18)</f>
-        <v>-1, 0, 0, 0, 0, 1, 0, 0, 0, 0, -1, 0, 0, 0, 0, 1</v>
+        <f>"=matrix3d(" &amp; _xlfn.TEXTJOIN(", ", TRUE,I15:L18) &amp; ")"</f>
+        <v>=matrix3d(-1, 0, 0, 0, 0, 1, 0, 0, 0, 0, -1, 0, 0, 0, 0, 1)</v>
       </c>
       <c r="J19" s="11"/>
       <c r="K19" s="11"/>
       <c r="L19" s="11"/>
       <c r="M19" s="1"/>
       <c r="N19" s="11" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE,N15:Q18)</f>
-        <v>-1, 0, 0, 0, 0, -1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1</v>
+        <f>"=matrix3d(" &amp; _xlfn.TEXTJOIN(", ", TRUE,N15:Q18) &amp; ")"</f>
+        <v>=matrix3d(-1, 0, 0, 0, 0, -1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1)</v>
       </c>
       <c r="O19" s="11"/>
       <c r="P19" s="11"/>
@@ -1652,24 +1748,24 @@
       <c r="A25" s="1"/>
       <c r="C25" s="10"/>
       <c r="D25" s="11" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE,D21:G24)</f>
-        <v>1, 0, 0, 0, 0, 0, -1, 0, 0, 1, 0, 0, 0, 0, 0, 1</v>
+        <f>"=matrix3d(" &amp; _xlfn.TEXTJOIN(", ", TRUE,D21:G24) &amp; ")"</f>
+        <v>=matrix3d(1, 0, 0, 0, 0, 0, -1, 0, 0, 1, 0, 0, 0, 0, 0, 1)</v>
       </c>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
       <c r="H25" s="1"/>
       <c r="I25" s="11" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE,I21:L24)</f>
-        <v>0, 0, 1, 0, 0, 1, 0, 0, -1, 0, 0, 0, 0, 0, 0, 1</v>
+        <f>"=matrix3d(" &amp; _xlfn.TEXTJOIN(", ", TRUE,I21:L24) &amp; ")"</f>
+        <v>=matrix3d(0, 0, 1, 0, 0, 1, 0, 0, -1, 0, 0, 0, 0, 0, 0, 1)</v>
       </c>
       <c r="J25" s="11"/>
       <c r="K25" s="11"/>
       <c r="L25" s="11"/>
       <c r="M25" s="1"/>
       <c r="N25" s="11" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE,N21:Q24)</f>
-        <v>0, -1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1</v>
+        <f>"=matrix3d(" &amp; _xlfn.TEXTJOIN(", ", TRUE,N21:Q24) &amp; ")"</f>
+        <v>=matrix3d(0, -1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1)</v>
       </c>
       <c r="O25" s="11"/>
       <c r="P25" s="11"/>
@@ -1907,24 +2003,24 @@
       <c r="A31" s="1"/>
       <c r="C31" s="10"/>
       <c r="D31" s="11" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE,D27:G30)</f>
-        <v>1, 0, 0, 0, 0, 0, 1, 0, 0, -1, 0, 0, 0, 0, 0, 1</v>
+        <f>"=matrix3d(" &amp; _xlfn.TEXTJOIN(", ", TRUE,D27:G30) &amp; ")"</f>
+        <v>=matrix3d(1, 0, 0, 0, 0, 0, 1, 0, 0, -1, 0, 0, 0, 0, 0, 1)</v>
       </c>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
       <c r="H31" s="1"/>
       <c r="I31" s="11" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE,I27:L30)</f>
-        <v>0, 0, -1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1</v>
+        <f>"=matrix3d(" &amp; _xlfn.TEXTJOIN(", ", TRUE,I27:L30) &amp; ")"</f>
+        <v>=matrix3d(0, 0, -1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1)</v>
       </c>
       <c r="J31" s="11"/>
       <c r="K31" s="11"/>
       <c r="L31" s="11"/>
       <c r="M31" s="1"/>
       <c r="N31" s="11" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE,N27:Q30)</f>
-        <v>0, 1, 0, 0, -1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1</v>
+        <f>"=matrix3d(" &amp; _xlfn.TEXTJOIN(", ", TRUE,N27:Q30) &amp; ")"</f>
+        <v>=matrix3d(0, 1, 0, 0, -1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1)</v>
       </c>
       <c r="O31" s="11"/>
       <c r="P31" s="11"/>
@@ -1938,6 +2034,10 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="N13:Q13"/>
     <mergeCell ref="D31:G31"/>
     <mergeCell ref="I31:L31"/>
     <mergeCell ref="N31:Q31"/>
@@ -1947,29 +2047,15 @@
     <mergeCell ref="D25:G25"/>
     <mergeCell ref="I25:L25"/>
     <mergeCell ref="N25:Q25"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="N13:Q13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D9:Q12 D13 H13 D14:Q18 M13 D20:Q24 D26:Q30">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="25" operator="lessThan">
       <formula>-0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="lessThan">
-      <formula>-0.1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I19">
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="lessThan">
-      <formula>-0.1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I25">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="lessThan">
       <formula>-0.1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1983,13 +2069,23 @@
       <formula>-0.1</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I19">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
+      <formula>-0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="N19">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThan">
       <formula>-0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25 H25 M25">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
+      <formula>-0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
       <formula>-0.1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1998,13 +2094,13 @@
       <formula>-0.1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I31">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+  <conditionalFormatting sqref="D31 H31 M31">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>-0.1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31 H31 M31">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
+  <conditionalFormatting sqref="I31">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>-0.1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2013,7 +2109,8 @@
       <formula>-0.1</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>